<commit_message>
finalization of implementation of alpha_fixé_gamma_H0_OmegaM
</commit_message>
<xml_diff>
--- a/2-modèle G modifié/calibration/2_Modèle uniquement/Résultats (intervalle confiance 68%).xlsx
+++ b/2-modèle G modifié/calibration/2_Modèle uniquement/Résultats (intervalle confiance 68%).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero 3A 2023-2024\projet recherche\travail concret projet\2-modèle G modifié\calibration\2_Modèle uniquement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero_3A_2023-2024\projet_recherche\travail_concret_projet\2-modèle G modifié\calibration\2_Modèle uniquement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4870B625-CC9C-44AF-9FFC-0EEDFCE1B593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836260D0-0EE9-4535-90BB-67ED7C8F994A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>only alpha</t>
   </si>
@@ -81,30 +81,37 @@
   </si>
   <si>
     <t>alpha_fixé_gamma_exp</t>
+  </si>
+  <si>
+    <t>H0</t>
+  </si>
+  <si>
+    <t>Omegam</t>
+  </si>
+  <si>
+    <t>alpha_fixé_H0_Omegam</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>73, 3</t>
+  </si>
+  <si>
+    <t>alpha_fixé_H0 (alpha = 0,18 )</t>
+  </si>
+  <si>
+    <t>alpha_fixé_H0 (alpha_brout_f_lcdm = 0.192)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,10 +137,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,28 +420,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="69" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="11" max="11" width="17.140625" customWidth="1"/>
     <col min="12" max="12" width="21.28515625" customWidth="1"/>
     <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="107.5703125" customWidth="1"/>
+    <col min="14" max="14" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -444,7 +450,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -453,7 +459,7 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -462,142 +468,233 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="H2">
         <v>-8.9999999999997807E-3</v>
       </c>
-      <c r="C2">
-        <f>ABS(B2-(-0.00599999999999978))</f>
+      <c r="I2">
+        <f>ABS(H2-(-0.00599999999999978))</f>
         <v>3.0000000000000009E-3</v>
       </c>
-      <c r="D2">
-        <f>ABS(B2-(-0.0119999999999997))</f>
+      <c r="J2">
+        <f>ABS(H2-(-0.0119999999999997))</f>
         <v>2.9999999999999194E-3</v>
       </c>
-      <c r="K2">
+      <c r="Q2">
         <v>1523.03995256948</v>
       </c>
-      <c r="L2">
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="M2">
-        <f>K2+L2*2</f>
+      <c r="S2">
+        <f>Q2+R2*2</f>
         <v>1525.03995256948</v>
       </c>
-      <c r="N2" t="s">
+      <c r="T2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
+      <c r="H3">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="C3">
-        <f>ABS(B3-(-0.00999999999999978))</f>
+      <c r="I3">
+        <f>ABS(H3-(-0.00999999999999978))</f>
         <v>9.9999999999978058E-4</v>
       </c>
-      <c r="D3">
-        <f>ABS(B3-(-0.0119999999999997))</f>
+      <c r="J3">
+        <f>ABS(H3-(-0.0119999999999997))</f>
         <v>2.9999999999997008E-3</v>
       </c>
-      <c r="H3">
+      <c r="N3">
         <v>-3.99999999999998E-2</v>
       </c>
-      <c r="I3">
-        <f>ABS(H3-(-0.0599999999999998))</f>
+      <c r="O3">
+        <f>ABS(N3-(-0.0599999999999998))</f>
         <v>1.9999999999999997E-2</v>
       </c>
-      <c r="J3">
-        <f>ABS(H3-(-0.00999999999999978))</f>
+      <c r="P3">
+        <f>ABS(N3-(-0.00999999999999978))</f>
         <v>3.000000000000002E-2</v>
       </c>
-      <c r="K3">
+      <c r="Q3">
         <v>1522.6266523066399</v>
       </c>
-      <c r="L3">
+      <c r="R3">
         <v>2</v>
       </c>
-      <c r="M3">
-        <f>K3+L3*2</f>
+      <c r="S3">
+        <f>Q3+R3*2</f>
         <v>1526.6266523066399</v>
       </c>
-      <c r="N3" t="s">
+      <c r="T3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="H4">
+      <c r="N4">
         <v>-9.9999999999955593E-4</v>
       </c>
-      <c r="I4" t="s">
+      <c r="O4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" t="s">
+      <c r="P4" t="s">
         <v>9</v>
       </c>
-      <c r="K4">
+      <c r="Q4">
         <v>1536.6936363135401</v>
       </c>
-      <c r="L4">
+      <c r="R4">
         <v>1</v>
       </c>
-      <c r="M4">
-        <f>K4+L4*2</f>
+      <c r="S4">
+        <f>Q4+R4*2</f>
         <v>1538.6936363135401</v>
       </c>
-      <c r="N4" t="s">
+      <c r="T4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="E5">
+      <c r="K5">
         <v>-4.5999999999999902E-2</v>
       </c>
-      <c r="F5">
-        <f>ABS(E5-(-0.0739999999999999))</f>
+      <c r="L5">
+        <f>ABS(K5-(-0.0739999999999999))</f>
         <v>2.7999999999999997E-2</v>
       </c>
-      <c r="G5">
-        <f>ABS(E5-(0.0179999999999999))</f>
+      <c r="M5">
+        <f>ABS(K5-(0.0179999999999999))</f>
         <v>6.3999999999999807E-2</v>
       </c>
-      <c r="K5">
+      <c r="Q5">
         <v>1523.01313790014</v>
       </c>
-      <c r="L5">
+      <c r="R5">
         <v>1</v>
       </c>
-      <c r="M5">
-        <f>K5+L5*2</f>
+      <c r="S5">
+        <f>Q5+R5*2</f>
         <v>1525.01313790014</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6:S8" si="0">Q6+R6*2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="C7">
+        <f>ABS(B7-68.0270000000072)</f>
+        <v>0.12700000000720024</v>
+      </c>
+      <c r="D7">
+        <f>ABS(B7-67.799)</f>
+        <v>0.10099999999999909</v>
+      </c>
+      <c r="Q7">
+        <v>1527.9420679014299</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>1529.9420679014299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="C8">
+        <f>ABS(B8-67.7090000000057)</f>
+        <v>0.10900000000570742</v>
+      </c>
+      <c r="D8">
+        <f>ABS(B8-67.4820000000046)</f>
+        <v>0.11799999999539068</v>
+      </c>
+      <c r="Q8">
+        <v>1528.5330347676099</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>1530.5330347676099</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
replacement of Z, CL_68 and CL_95 by Chi2,CI_1σ and CI_2σ in the programmes + replacement of deltachi2 = 3.841 by 4 in case of 1 parameter for CI_68
</commit_message>
<xml_diff>
--- a/2-modèle G modifié/calibration/2_Modèle uniquement/Résultats (intervalle confiance 68%).xlsx
+++ b/2-modèle G modifié/calibration/2_Modèle uniquement/Résultats (intervalle confiance 68%).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero_3A_2023-2024\projet_recherche\travail_concret_projet\2-modèle G modifié\calibration\2_Modèle uniquement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836260D0-0EE9-4535-90BB-67ED7C8F994A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE1D3A8-CA58-4653-AD3D-2E930609B44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>only alpha</t>
   </si>
@@ -90,12 +90,6 @@
   </si>
   <si>
     <t>alpha_fixé_H0_Omegam</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>73, 3</t>
   </si>
   <si>
     <t>alpha_fixé_H0 (alpha = 0,18 )</t>
@@ -422,14 +416,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="69" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
@@ -621,32 +616,42 @@
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
+      <c r="B6">
+        <v>73.3</v>
+      </c>
+      <c r="C6">
+        <f>ABS(B6-73.6)</f>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="D6">
+        <f>ABS(B6-72.9999999999995)</f>
+        <v>0.30000000000049454</v>
       </c>
       <c r="E6">
         <v>0.28599999999999998</v>
       </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
+      <c r="F6">
+        <f>ABS(E6-0.314)</f>
+        <v>2.8000000000000025E-2</v>
+      </c>
+      <c r="G6">
+        <f>ABS(E6-0.264)</f>
+        <v>2.1999999999999964E-2</v>
+      </c>
+      <c r="Q6">
+        <v>1522.7850747291</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
       </c>
       <c r="S6">
         <f t="shared" ref="S6:S8" si="0">Q6+R6*2</f>
-        <v>0</v>
+        <v>1526.7850747291</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>67.900000000000006</v>
@@ -672,7 +677,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>67.599999999999994</v>

</xml_diff>

<commit_message>
avancée tentative de parallélisation
</commit_message>
<xml_diff>
--- a/2-modèle G modifié/calibration/2_Modèle uniquement/Résultats (intervalle confiance 68%).xlsx
+++ b/2-modèle G modifié/calibration/2_Modèle uniquement/Résultats (intervalle confiance 68%).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero_3A_2023-2024\projet_recherche\travail_concret_projet\2-modèle G modifié\calibration\2_Modèle uniquement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE1D3A8-CA58-4653-AD3D-2E930609B44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2C0E73-611F-4C4D-BA04-E5AF98B61135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>only alpha</t>
   </si>
@@ -89,13 +89,16 @@
     <t>Omegam</t>
   </si>
   <si>
-    <t>alpha_fixé_H0_Omegam</t>
-  </si>
-  <si>
     <t>alpha_fixé_H0 (alpha = 0,18 )</t>
   </si>
   <si>
     <t>alpha_fixé_H0 (alpha_brout_f_lcdm = 0.192)</t>
+  </si>
+  <si>
+    <t>alpha_fixé_H0_Omegam (alpha = 0,18 )</t>
+  </si>
+  <si>
+    <t>alpha_fixé_H0_Omegam  (alpha_brout_f_lcdm = 0.192)</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +617,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>73.3</v>
@@ -645,59 +648,64 @@
         <v>2</v>
       </c>
       <c r="S6">
-        <f t="shared" ref="S6:S8" si="0">Q6+R6*2</f>
+        <f t="shared" ref="S6" si="0">Q6+R6*2</f>
         <v>1526.7850747291</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>67.900000000000006</v>
-      </c>
-      <c r="C7">
-        <f>ABS(B7-68.0270000000072)</f>
-        <v>0.12700000000720024</v>
-      </c>
-      <c r="D7">
-        <f>ABS(B7-67.799)</f>
-        <v>0.10099999999999909</v>
-      </c>
-      <c r="Q7">
-        <v>1527.9420679014299</v>
-      </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="0"/>
-        <v>1529.9420679014299</v>
+      <c r="A7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8">
-        <v>67.599999999999994</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="C8">
-        <f>ABS(B8-67.7090000000057)</f>
-        <v>0.10900000000570742</v>
+        <f>ABS(B8-68.0270000000072)</f>
+        <v>0.12700000000720024</v>
       </c>
       <c r="D8">
-        <f>ABS(B8-67.4820000000046)</f>
-        <v>0.11799999999539068</v>
+        <f>ABS(B8-67.799)</f>
+        <v>0.10099999999999909</v>
       </c>
       <c r="Q8">
-        <v>1528.5330347676099</v>
+        <v>1527.9420679014299</v>
       </c>
       <c r="R8">
         <v>1</v>
       </c>
       <c r="S8">
-        <f t="shared" si="0"/>
+        <f>Q8+R8*2</f>
+        <v>1529.9420679014299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="C9">
+        <f>ABS(B9-67.7090000000057)</f>
+        <v>0.10900000000570742</v>
+      </c>
+      <c r="D9">
+        <f>ABS(B9-67.4820000000046)</f>
+        <v>0.11799999999539068</v>
+      </c>
+      <c r="Q9">
+        <v>1528.5330347676099</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <f>Q9+R9*2</f>
         <v>1530.5330347676099</v>
       </c>
     </row>

</xml_diff>